<commit_message>
add dumbbell chart directions
</commit_message>
<xml_diff>
--- a/data/charts.xlsx
+++ b/data/charts.xlsx
@@ -8,18 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shenyue/Documents/GitHub/data-viz-non-coders-boot-camp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2A2927-1A8A-A444-906D-6064D92F7667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3270BB-CFC6-D641-B6B2-42E714D803DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22700" yWindow="2400" windowWidth="27640" windowHeight="16940" xr2:uid="{539DB220-64E6-144D-868E-749D6BD0C0B1}"/>
+    <workbookView xWindow="3280" yWindow="500" windowWidth="30180" windowHeight="16940" activeTab="1" xr2:uid="{539DB220-64E6-144D-868E-749D6BD0C0B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Bar Plot" sheetId="1" r:id="rId1"/>
+    <sheet name="Dumbbell" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Dumbbell!$B$3</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Dumbbell!$B$4:$B$11</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Dumbbell!$C$3</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Dumbbell!$C$4:$C$11</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Dumbbell!$D$4:$D$11</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Dumbbell!$B$3</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Dumbbell!$B$4:$B$11</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Dumbbell!$C$3</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Dumbbell!$C$4:$C$11</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Dumbbell!$D$4:$D$11</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Manufacturing company sourcing parts from Chine &amp; US</t>
   </si>
@@ -67,12 +79,64 @@
   <si>
     <t>HPC chips</t>
   </si>
+  <si>
+    <t>Employee Engagement Scores based on internal surveys</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Engagement Score in 2023 (%)</t>
+  </si>
+  <si>
+    <t>Engagement Score in 2024 (%)</t>
+  </si>
+  <si>
+    <t>y-position</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>labels</t>
+  </si>
+  <si>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>Customer Service</t>
+  </si>
+  <si>
+    <t>Operations</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Procurement</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -89,12 +153,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -115,16 +185,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -214,7 +293,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'[2]Template Chart 1'!$B$5</c:f>
+              <c:f>'[1]Template Chart 1'!$B$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -290,7 +369,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'[2]Template Chart 1'!$A$6:$A$10</c:f>
+              <c:f>'[1]Template Chart 1'!$A$6:$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -313,7 +392,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'[2]Template Chart 1'!$B$6:$B$10</c:f>
+              <c:f>'[1]Template Chart 1'!$B$6:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -346,7 +425,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'[2]Template Chart 1'!$C$5</c:f>
+              <c:f>'[1]Template Chart 1'!$C$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -427,7 +506,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'[2]Template Chart 1'!$A$6:$A$10</c:f>
+              <c:f>'[1]Template Chart 1'!$A$6:$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -450,7 +529,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'[2]Template Chart 1'!$C$6:$C$10</c:f>
+              <c:f>'[1]Template Chart 1'!$C$6:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -618,7 +697,533 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Dumbbell!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Engagement Score in 2023 (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Dumbbell!$B$4:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Dumbbell!$D$4:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7D78-1E4F-BCB9-2D35DF9F15BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Dumbbell!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Engagement Score in 2024 (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="minus"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="1"/>
+            <c:plus>
+              <c:numLit>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numLit>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Dumbbell!$E$4:$E$11</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="8"/>
+                  <c:pt idx="0">
+                    <c:v>0.14999999999999997</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>9.9999999999999978E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>-0.10000000000000009</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>-6.9999999999999951E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.10000000000000003</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.23000000000000004</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>5.0000000000000044E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>5.0000000000000044E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Dumbbell!$C$4:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Dumbbell!$D$4:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7D78-1E4F-BCB9-2D35DF9F15BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="227320528"/>
+        <c:axId val="227322256"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="227320528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="227322256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="227322256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="227320528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1163,6 +1768,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1170,13 +2291,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>139700</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>142115</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>148501</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>127001</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1249,6 +2370,7 @@
               <a:latin typeface="Calibri"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
+            <a:pPr/>
             <a:t>Battery cells</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100"/>
@@ -1297,6 +2419,7 @@
               <a:latin typeface="Calibri"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
+            <a:pPr/>
             <a:t>Microprocessors</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100"/>
@@ -1345,6 +2468,7 @@
               <a:latin typeface="Calibri"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
+            <a:pPr/>
             <a:t>LCD Displays</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100"/>
@@ -1393,6 +2517,7 @@
               <a:latin typeface="Calibri"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
+            <a:pPr/>
             <a:t>Sensors</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100"/>
@@ -1441,6 +2566,7 @@
               <a:latin typeface="Calibri"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
+            <a:pPr/>
             <a:t>HPC chips</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100"/>
@@ -1451,20 +2577,48 @@
 </c:userShapes>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Template Chart 1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>44450</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>488950</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5712BFB-86DF-B1DB-FDD4-5D5278758413}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -1482,11 +2636,6 @@
       <sheetData sheetId="0"/>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2">
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>Parts sourced from China and United States</v>
-          </cell>
-        </row>
         <row r="5">
           <cell r="B5" t="str">
             <v>China</v>
@@ -1858,8 +3007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7FF0F3-76EE-1442-A5FB-43B60D4EC0AE}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1941,4 +3090,215 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44FC017-7051-7849-AD89-31D5543876C8}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.35</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7">
+        <f>C4-B4</f>
+        <v>0.14999999999999997</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="D5" s="5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="7">
+        <f t="shared" ref="E5:E11" si="0">C5-B5</f>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="D6" s="5">
+        <v>3</v>
+      </c>
+      <c r="E6" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.10000000000000009</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.78</v>
+      </c>
+      <c r="D7" s="5">
+        <v>4</v>
+      </c>
+      <c r="E7" s="7">
+        <f t="shared" si="0"/>
+        <v>-6.9999999999999951E-2</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0.45</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D8" s="5">
+        <v>5</v>
+      </c>
+      <c r="E8" s="7">
+        <f t="shared" si="0"/>
+        <v>0.10000000000000003</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0.32</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D9" s="5">
+        <v>6</v>
+      </c>
+      <c r="E9" s="7">
+        <f t="shared" si="0"/>
+        <v>0.23000000000000004</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0.65</v>
+      </c>
+      <c r="D10" s="5">
+        <v>7</v>
+      </c>
+      <c r="E10" s="7">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="D11" s="5">
+        <v>8</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update dumbbell chart directions
</commit_message>
<xml_diff>
--- a/data/charts.xlsx
+++ b/data/charts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shenyue/Documents/GitHub/data-viz-non-coders-boot-camp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3270BB-CFC6-D641-B6B2-42E714D803DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A9AD06-45DF-F645-A44F-9BA4A0E171BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3280" yWindow="500" windowWidth="30180" windowHeight="16940" activeTab="1" xr2:uid="{539DB220-64E6-144D-868E-749D6BD0C0B1}"/>
+    <workbookView xWindow="40" yWindow="500" windowWidth="15200" windowHeight="18720" activeTab="1" xr2:uid="{539DB220-64E6-144D-868E-749D6BD0C0B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Bar Plot" sheetId="1" r:id="rId1"/>
@@ -19,18 +19,6 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Dumbbell!$B$3</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Dumbbell!$B$4:$B$11</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Dumbbell!$C$3</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Dumbbell!$C$4:$C$11</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Dumbbell!$D$4:$D$11</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Dumbbell!$B$3</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Dumbbell!$B$4:$B$11</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Dumbbell!$C$3</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Dumbbell!$C$4:$C$11</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Dumbbell!$D$4:$D$11</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -80,9 +68,6 @@
     <t>HPC chips</t>
   </si>
   <si>
-    <t>Employee Engagement Scores based on internal surveys</t>
-  </si>
-  <si>
     <t>Department</t>
   </si>
   <si>
@@ -123,6 +108,9 @@
   </si>
   <si>
     <t>HR</t>
+  </si>
+  <si>
+    <t>Employee Engagement Scoresfrom 2023 to 2024</t>
   </si>
 </sst>
 </file>
@@ -711,9 +699,97 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Employee Engagement Scores from </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="40000"/>
+                    <a:lumOff val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>2023</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t> to </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>2024</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18568440791802607"/>
+          <c:y val="0.14814814814814814"/>
+          <c:w val="0.76868380516833934"/>
+          <c:h val="0.74445246427529888"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -740,15 +816,16 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="7"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -849,7 +926,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="7"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
@@ -911,11 +988,10 @@
             </c:minus>
             <c:spPr>
               <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:round/>
@@ -993,6 +1069,464 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-7D78-1E4F-BCB9-2D35DF9F15BB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>labels</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{FE551614-03D7-B545-AA07-62259A84A203}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="l"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-24C9-FE43-AFF5-09AE16229B90}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{72B4FEE9-A4A2-F041-B00B-0013B9148472}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="l"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-24C9-FE43-AFF5-09AE16229B90}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{B05F62A5-E8AC-5640-9948-FC84A293282B}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="l"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-24C9-FE43-AFF5-09AE16229B90}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{DF239DE4-3B72-7F4F-844E-AAA53D4801D9}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="l"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-24C9-FE43-AFF5-09AE16229B90}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{19BD8D5C-775D-4744-9FDD-B43462354551}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="l"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-24C9-FE43-AFF5-09AE16229B90}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{67EB1E89-0FCF-F845-8955-9B5B59B5C3B9}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="l"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-24C9-FE43-AFF5-09AE16229B90}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{183E4D83-76AC-5C48-A531-801D43A41D37}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="l"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-24C9-FE43-AFF5-09AE16229B90}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{90440CD2-C360-5940-BF20-87923C882EDA}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="l"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-24C9-FE43-AFF5-09AE16229B90}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="l"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Dumbbell!$F$4:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Dumbbell!$D$4:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>Dumbbell!$A$4:$A$11</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="8"/>
+                  <c:pt idx="0">
+                    <c:v>Production</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Finance</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Customer Service</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Operations</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>IT</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Procurement</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Sales</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>HR</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-24C9-FE43-AFF5-09AE16229B90}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1018,9 +1552,8 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1057,9 +1590,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -1074,15 +1607,14 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1094,39 +1626,6 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="227320528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -1170,7 +1669,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -2581,16 +3083,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>44450</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>488950</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3097,41 +3599,41 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
     <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="6">
         <v>0.2</v>
@@ -3152,7 +3654,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="6">
         <v>0.6</v>
@@ -3173,7 +3675,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="6">
         <v>0.8</v>
@@ -3194,7 +3696,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="6">
         <v>0.85</v>
@@ -3215,7 +3717,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="6">
         <v>0.45</v>
@@ -3236,7 +3738,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="6">
         <v>0.32</v>
@@ -3257,7 +3759,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="6">
         <v>0.6</v>
@@ -3278,7 +3780,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="6">
         <v>0.75</v>

</xml_diff>